<commit_message>
add collector_id for export EF xlsx
</commit_message>
<xml_diff>
--- a/tests/unit/apps/payment/test_file/pp_payment_list_valid.xlsx
+++ b/tests/unit/apps/payment/test_file/pp_payment_list_valid.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>payment_id</t>
   </si>
@@ -19,6 +19,9 @@
     <t>household_id</t>
   </si>
   <si>
+    <t>collector_id</t>
+  </si>
+  <si>
     <t>household_size</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t>HH-20-0000.0001</t>
   </si>
   <si>
+    <t>IND-24-0000.0012</t>
+  </si>
+  <si>
     <t>Achin</t>
   </si>
   <si>
@@ -80,6 +86,9 @@
   </si>
   <si>
     <t>HH-20-0000.0002</t>
+  </si>
+  <si>
+    <t>IND-24-0000.0013</t>
   </si>
   <si>
     <t>Abband</t>
@@ -1518,23 +1527,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="38" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="5" width="13.1719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85156" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25" style="1" customWidth="1"/>
-    <col min="11" max="13" width="26.5" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" customWidth="1"/>
+    <col min="5" max="6" width="13.1719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85156" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="1" customWidth="1"/>
+    <col min="12" max="14" width="26.5" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1553,22 +1562,22 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="4">
+      <c r="G1" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="5">
+      <c r="H1" t="s" s="4">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="3">
+      <c r="I1" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="4">
+      <c r="J1" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="6">
+      <c r="K1" t="s" s="4">
         <v>10</v>
       </c>
       <c r="L1" t="s" s="6">
@@ -1576,82 +1585,91 @@
       </c>
       <c r="M1" t="s" s="6">
         <v>12</v>
+      </c>
+      <c r="N1" t="s" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C2" s="7">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s" s="4">
+      <c r="E2" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="H2" t="s" s="5">
+      <c r="F2" s="2"/>
+      <c r="G2" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="H2" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="J2" s="8">
+      <c r="I2" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K2" s="8">
         <v>99</v>
       </c>
-      <c r="K2" s="9">
+      <c r="L2" s="9">
         <v>3637</v>
       </c>
-      <c r="L2" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="M2" s="6"/>
+      <c r="M2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="K3" s="8">
+        <v>11.11</v>
+      </c>
+      <c r="L3" s="9">
+        <v>3589</v>
+      </c>
+      <c r="M3" t="s" s="6">
         <v>22</v>
       </c>
-      <c r="C3" s="7">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s" s="4">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s" s="5">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s" s="3">
-        <v>27</v>
-      </c>
-      <c r="J3" s="8">
-        <v>11.11</v>
-      </c>
-      <c r="K3" s="9">
-        <v>3589</v>
-      </c>
-      <c r="L3" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="M3" t="s" s="6">
-        <v>28</v>
+      <c r="N3" t="s" s="6">
+        <v>31</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
@@ -1661,13 +1679,14 @@
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
       <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="15"/>
@@ -1680,9 +1699,10 @@
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="18"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="17"/>
       <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="15"/>
@@ -1695,9 +1715,10 @@
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="17"/>
       <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="15"/>
@@ -1710,9 +1731,10 @@
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="18"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="17"/>
       <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="15"/>
@@ -1725,9 +1747,10 @@
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="17"/>
       <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="15"/>
@@ -1740,9 +1763,10 @@
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="18"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="17"/>
       <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="19"/>
@@ -1755,9 +1779,10 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="22"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="21"/>
       <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>